<commit_message>
* DatasetDef and DatasetData. Completed implementation using a simple test Spreadsheet and external CSV file. * Fix bug: "parse_command" * Fix bug: proper initialization of "level" property for a HierarchyNode * Minor refactoring (two functions into "helper.py")
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/07_custom_datasets.xlsx
+++ b/backend_tests/z_input_files/v2/07_custom_datasets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="82">
   <si>
     <t xml:space="preserve">Case study code</t>
   </si>
@@ -196,58 +196,97 @@
     <t xml:space="preserve">ConceptName</t>
   </si>
   <si>
-    <t xml:space="preserve">DataType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Domain</t>
+    <t xml:space="preserve">ConceptDataType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConceptDomain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">file:///</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">home/rnebot/GoogleDrive/AA_MAGIC/nis-backend/backend_tests/z_input_files/v2/07_custom_dataset_test1.csv</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Test dataset #1</t>
   </si>
   <si>
     <t xml:space="preserve">Dimension</t>
   </si>
   <si>
-    <t xml:space="preserve">Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hierarchy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISO3166 codes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL_Countries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key-value list</t>
+    <t xml:space="preserve">Geo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Hierarchy</t>
   </si>
   <si>
     <t xml:space="preserve">Measure</t>
   </si>
   <si>
-    <t xml:space="preserve">TotalFood</t>
+    <t xml:space="preserve">Surface</t>
   </si>
   <si>
     <t xml:space="preserve">Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Total mass food per country</t>
+    <t xml:space="preserve">Category surface</t>
   </si>
   <si>
     <t xml:space="preserve">Attribute</t>
   </si>
   <si>
-    <t xml:space="preserve">TotalFoodUnit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tonnes or Calories?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concept1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concept2</t>
+    <t xml:space="preserve">SurfaceUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UnitName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Either km2 or SquareMile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data://</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test dataset #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PopulationDensity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Either p/km2 or p/SquareMile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km2</t>
   </si>
 </sst>
 </file>
@@ -257,7 +296,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -285,6 +324,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -329,7 +381,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -359,6 +411,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -531,7 +591,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -737,19 +797,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -796,27 +859,21 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="7" t="s">
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -836,23 +893,25 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="7" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="G3" s="0" t="s">
+        <v>37</v>
+      </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -872,23 +931,22 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="7" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -908,7 +966,129 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="file:///"/>
+    <hyperlink ref="B6" r:id="rId2" display="data://"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -924,27 +1104,88 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>74</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Syntax validation, help system, list of datasets
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/07_custom_datasets.xlsx
+++ b/backend_tests/z_input_files/v2/07_custom_datasets.xlsx
@@ -205,7 +205,7 @@
     <t xml:space="preserve">test1</t>
   </si>
   <si>
-    <t xml:space="preserve">file:///tmp/07_custom_dataset_test1.csv</t>
+    <t xml:space="preserve">file:///home/rnebot/GoogleDrive/AA_MAGIC/nis-backend/backend_tests/z_input_files/v2/07_custom_dataset_test1.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Test dataset #1</t>
@@ -393,12 +393,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -547,8 +547,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -755,8 +755,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1055,15 +1055,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="file:///tmp/07_custom_dataset_test1.csv"/>
+    <hyperlink ref="B2" r:id="rId1" display="file:///home/rnebot/GoogleDrive/AA_MAGIC/nis-backend/backend_tests/z_input_files/v2/07_custom_dataset_test1.csv"/>
     <hyperlink ref="B6" r:id="rId2" display="data://"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1162,8 +1162,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ScalarBenchmarks command, Benchmark class
* Specification of Benchmarks
* Rearranging order of (and disabling) commands (this order appears in the NIS-frontend)
* ScalarIndicators reads the Benchmark if it is specified
* "number_interval" parser carrying modification to several "pyparsing" rules
* Metadata command: "global" as new category for the Geographical Level of a Case Study
* Return issues to frontend prefixed with the Issue type (Error, Warning, Info) so that the type is shown to the user
* New test workbook for dataset expansion
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/07_custom_datasets.xlsx
+++ b/backend_tests/z_input_files/v2/07_custom_datasets.xlsx
@@ -47,13 +47,13 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Case study specifying test datasets with the only purpose of testing the application</t>
+    <t xml:space="preserve">Case study specifying test datasets with the only purpose of testing</t>
   </si>
   <si>
     <t xml:space="preserve">Geographical level</t>
   </si>
   <si>
-    <t xml:space="preserve">Regional</t>
+    <t xml:space="preserve">Global</t>
   </si>
   <si>
     <t xml:space="preserve">Dimensions</t>
@@ -83,7 +83,7 @@
     <t xml:space="preserve">Geographical location</t>
   </si>
   <si>
-    <t xml:space="preserve">Almería</t>
+    <t xml:space="preserve">Cyberworld</t>
   </si>
   <si>
     <t xml:space="preserve">DOI</t>
@@ -251,7 +251,7 @@
     <t xml:space="preserve">https://nextcloud.data.magic-nexus.eu/remote.php/webdav/NIS_beta/CS_format_examples/07_custom_dataset_test1_external.xlsx#Worksheet_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Test dataset #5. External, stored in Nextcloud of MAGIC project, XLSX format (pointing to one of the worksheets)</t>
+    <t xml:space="preserve">Test dataset #5. External, stored in Nextcloud of MAGIC project, XLSX format &amp; pointing to one of the worksheets</t>
   </si>
   <si>
     <t xml:space="preserve">Surface</t>
@@ -439,7 +439,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -797,7 +797,7 @@
   <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -805,9 +805,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="100.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="57.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="94.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.39"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
@@ -918,7 +918,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="11.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>73</v>
       </c>
@@ -1060,7 +1060,7 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
         <v>80</v>
       </c>

</xml_diff>